<commit_message>
every new search will create separate tab with days and time, added read me file
</commit_message>
<xml_diff>
--- a/excel_file/updated_keywords.xlsx
+++ b/excel_file/updated_keywords.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Wednesday" sheetId="1" r:id="rId1"/>
+    <sheet name="Thursday_112352" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -28,7 +28,7 @@
     <t>EPL</t>
   </si>
   <si>
-    <t>Premier League News - Results, Fixtures, Scores, Stats ...</t>
+    <t>Premier League Football - Latest news, results, stats ... - BBC</t>
   </si>
   <si>
     <t>Clubs</t>
@@ -52,7 +52,7 @@
     <t>seria A</t>
   </si>
   <si>
-    <t>Serie A News - Results, Fixtures, Scores, Stats, and Rumors</t>
+    <t>Serie A Table - Football - BBC Sport</t>
   </si>
   <si>
     <t>Serie A</t>

</xml_diff>